<commit_message>
Actualizacion titulo web y notas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mi unidad\2025 Mate Pi\consulta_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB34433C-B093-40E4-8E9F-4E9380B04373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03515325-C18A-4C49-953F-437234DDC9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="5">
   <si>
     <t>B0244942</t>
   </si>
@@ -55,12 +55,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,8 +88,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -303,1021 +312,1024 @@
   <dimension ref="A1:B128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="10.90625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>45502425</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>2.4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>41955136</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>32394029</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>46895985</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>96387711</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>96424700</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>43318864</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>96165363</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>46897686</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>45868089</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>43103633</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>96434389</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>96114027</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>40930816</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>96372729</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>44589822</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>4.7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>44462273</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>44052565</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>46353055</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>43798375</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>44824353</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>39406172</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>47643306</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>43463092</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>45166865</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>2.6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>45815891</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>47221686</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>1.8</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>46264268</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>94917262</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>44267224</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>47238373</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>44677808</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>46199184</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>95126334</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>45228227</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>34119786</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B39" t="s">
-        <v>2</v>
+      <c r="B39" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>95342174</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>44239243</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>47743497</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>27589461</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>2.1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>44592762</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>47230559</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>45517883</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>46640802</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>44464008</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>32952001</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>32533045</v>
       </c>
-      <c r="B50" t="s">
-        <v>2</v>
+      <c r="B50" s="2">
+        <v>1.2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>40076846</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>43859957</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>95133388</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>44890922</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>44885554</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>46939844</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>95424009</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>94958338</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="A60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="A61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>2</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="A62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="A63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="A64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="A65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="A66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="A67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="A68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="A69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="A70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="A71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="A72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="A73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="A74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="A75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="A76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="A77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>2</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="A78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="A79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="A80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="A81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" t="s">
+      <c r="A82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="A83" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="A84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="A85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="A86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="A87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="A88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="A89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="A90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="A91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="A92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="A93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="A94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="A95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="A96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" t="s">
+      <c r="A97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" t="s">
+      <c r="A98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" t="s">
+      <c r="A99" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>2</v>
-      </c>
-      <c r="B100" t="s">
+      <c r="A100" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" t="s">
+      <c r="A101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="A102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" t="s">
+      <c r="A103" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>2</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="A104" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" t="s">
+      <c r="A105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" t="s">
+      <c r="A106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" t="s">
+      <c r="A107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" t="s">
+      <c r="A108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="A109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>2</v>
-      </c>
-      <c r="B110" t="s">
+      <c r="A110" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" t="s">
+      <c r="A111" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" t="s">
+      <c r="A112" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" t="s">
+      <c r="A113" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" t="s">
+      <c r="A114" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" t="s">
+      <c r="A115" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" t="s">
+      <c r="A116" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>2</v>
-      </c>
-      <c r="B117" t="s">
+      <c r="A117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" t="s">
+      <c r="A118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" t="s">
+      <c r="A119" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
-        <v>2</v>
-      </c>
-      <c r="B120" t="s">
+      <c r="A120" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" t="s">
+      <c r="A121" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
-        <v>2</v>
-      </c>
-      <c r="B122" t="s">
+      <c r="A122" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" t="s">
+      <c r="A123" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" t="s">
+      <c r="A124" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>2</v>
-      </c>
-      <c r="B125" t="s">
+      <c r="A125" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" t="s">
+      <c r="A126" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B128">
+      <c r="B128" s="1">
         <v>15</v>
       </c>
     </row>

</xml_diff>